<commit_message>
added in equation for ostracoda and redid plots
</commit_message>
<xml_diff>
--- a/Raw_data/length_weight.xlsx
+++ b/Raw_data/length_weight.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bop22abs/Documents/PhD/Chapter_1_code/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F66D050-8E90-1642-960B-8DB7C7B3AFB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA953C6-18E3-8D41-AA2C-BCD776C112B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" activeTab="1" xr2:uid="{C220307A-61A0-7548-B4BF-B7957B87512F}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{C220307A-61A0-7548-B4BF-B7957B87512F}"/>
   </bookViews>
   <sheets>
     <sheet name="crustacean_epa" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="rotifer_lw" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">crustacean_epa!$B$1:$B$103</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">crustacean_epa!$B$1:$B$104</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1310" uniqueCount="632">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1314" uniqueCount="634">
   <si>
     <t>info</t>
   </si>
@@ -1937,6 +1937,12 @@
   </si>
   <si>
     <t>ff.v</t>
+  </si>
+  <si>
+    <t>Ostracoda</t>
+  </si>
+  <si>
+    <t>BP5</t>
   </si>
 </sst>
 </file>
@@ -2326,10 +2332,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77BAEA40-6DAE-2544-8F9C-5E52DCA61FD7}">
-  <dimension ref="A1:F103"/>
+  <dimension ref="A1:F104"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="F114" sqref="F114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4399,8 +4405,29 @@
         <v>233</v>
       </c>
     </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>633</v>
+      </c>
+      <c r="B104" t="s">
+        <v>632</v>
+      </c>
+      <c r="C104">
+        <v>1.7512000000000001</v>
+      </c>
+      <c r="D104">
+        <v>2.653</v>
+      </c>
+      <c r="E104" t="s">
+        <v>233</v>
+      </c>
+      <c r="F104" t="s">
+        <v>233</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="B1:B103" xr:uid="{77BAEA40-6DAE-2544-8F9C-5E52DCA61FD7}"/>
+  <autoFilter ref="B1:B104" xr:uid="{77BAEA40-6DAE-2544-8F9C-5E52DCA61FD7}"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4409,7 +4436,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF60F91B-724F-5242-9800-AE268756E1B0}">
   <dimension ref="A1:M273"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
done prelim stats tests
</commit_message>
<xml_diff>
--- a/Raw_data/length_weight.xlsx
+++ b/Raw_data/length_weight.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bop22abs/Documents/PhD/Chapter_1_code/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE9DFD58-FF32-2547-8FF6-9DD209DB12BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9806D568-8ABB-3242-8151-33127BA1C481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25580" yWindow="-11660" windowWidth="25580" windowHeight="28300" activeTab="1" xr2:uid="{C220307A-61A0-7548-B4BF-B7957B87512F}"/>
+    <workbookView xWindow="3820" yWindow="740" windowWidth="25580" windowHeight="18380" activeTab="1" xr2:uid="{C220307A-61A0-7548-B4BF-B7957B87512F}"/>
   </bookViews>
   <sheets>
     <sheet name="crustacean_epa" sheetId="1" r:id="rId1"/>
@@ -4430,8 +4430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF60F91B-724F-5242-9800-AE268756E1B0}">
   <dimension ref="A1:K273"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A234" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H260" sqref="H260"/>
+    <sheetView tabSelected="1" topLeftCell="A256" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E276" sqref="E276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4724,7 +4724,7 @@
         <v>2</v>
       </c>
       <c r="F9">
-        <v>256</v>
+        <v>500</v>
       </c>
       <c r="G9">
         <v>1500</v>
@@ -12863,6 +12863,12 @@
       <c r="D254">
         <v>4</v>
       </c>
+      <c r="F254">
+        <v>80</v>
+      </c>
+      <c r="G254">
+        <v>120</v>
+      </c>
       <c r="K254">
         <v>0.1</v>
       </c>
@@ -12877,6 +12883,12 @@
       <c r="D255">
         <v>4</v>
       </c>
+      <c r="F255">
+        <v>64</v>
+      </c>
+      <c r="G255">
+        <v>200</v>
+      </c>
       <c r="K255">
         <v>0.1</v>
       </c>
@@ -12891,6 +12903,12 @@
       <c r="D256">
         <v>2</v>
       </c>
+      <c r="F256">
+        <v>500</v>
+      </c>
+      <c r="G256">
+        <v>1500</v>
+      </c>
       <c r="K256">
         <v>3.9E-2</v>
       </c>
@@ -12905,6 +12923,12 @@
       <c r="D257">
         <v>4</v>
       </c>
+      <c r="F257">
+        <v>82</v>
+      </c>
+      <c r="G257">
+        <v>418</v>
+      </c>
       <c r="K257">
         <v>0.1</v>
       </c>
@@ -12933,6 +12957,12 @@
       <c r="D259">
         <v>2</v>
       </c>
+      <c r="F259">
+        <v>94</v>
+      </c>
+      <c r="G259">
+        <v>80</v>
+      </c>
       <c r="K259">
         <v>0.1</v>
       </c>
@@ -12947,6 +12977,12 @@
       <c r="D260">
         <v>4</v>
       </c>
+      <c r="F260">
+        <v>119</v>
+      </c>
+      <c r="G260">
+        <v>316</v>
+      </c>
       <c r="K260">
         <v>0.1</v>
       </c>
@@ -12961,6 +12997,12 @@
       <c r="D261">
         <v>4</v>
       </c>
+      <c r="F261">
+        <v>70</v>
+      </c>
+      <c r="G261">
+        <v>252</v>
+      </c>
       <c r="K261">
         <v>0.1</v>
       </c>
@@ -12975,6 +13017,12 @@
       <c r="D262">
         <v>4</v>
       </c>
+      <c r="F262">
+        <v>102</v>
+      </c>
+      <c r="G262">
+        <v>363</v>
+      </c>
       <c r="K262">
         <v>0.1</v>
       </c>
@@ -12989,6 +13037,12 @@
       <c r="D263">
         <v>2</v>
       </c>
+      <c r="F263">
+        <v>160</v>
+      </c>
+      <c r="G263">
+        <v>400</v>
+      </c>
       <c r="K263">
         <v>0.1</v>
       </c>
@@ -13003,6 +13057,12 @@
       <c r="D264">
         <v>2</v>
       </c>
+      <c r="F264">
+        <v>294</v>
+      </c>
+      <c r="G264">
+        <v>459</v>
+      </c>
       <c r="K264">
         <v>0.1</v>
       </c>
@@ -13042,6 +13102,12 @@
       <c r="D267">
         <v>6</v>
       </c>
+      <c r="F267">
+        <v>114</v>
+      </c>
+      <c r="G267">
+        <v>154</v>
+      </c>
       <c r="K267">
         <v>0.1</v>
       </c>
@@ -13056,6 +13122,12 @@
       <c r="D268">
         <v>4</v>
       </c>
+      <c r="F268">
+        <v>130</v>
+      </c>
+      <c r="G268">
+        <v>612</v>
+      </c>
       <c r="K268">
         <v>0.1</v>
       </c>
@@ -13067,6 +13139,12 @@
       <c r="D269">
         <v>5</v>
       </c>
+      <c r="F269">
+        <v>68</v>
+      </c>
+      <c r="G269">
+        <v>246</v>
+      </c>
       <c r="K269">
         <v>0.1</v>
       </c>
@@ -13095,6 +13173,12 @@
       <c r="D271">
         <v>2</v>
       </c>
+      <c r="F271">
+        <v>0</v>
+      </c>
+      <c r="G271">
+        <v>550</v>
+      </c>
       <c r="K271">
         <v>0.1</v>
       </c>
@@ -13109,6 +13193,12 @@
       <c r="D272">
         <v>4</v>
       </c>
+      <c r="F272">
+        <v>90</v>
+      </c>
+      <c r="G272">
+        <v>258</v>
+      </c>
       <c r="K272">
         <v>0.1</v>
       </c>
@@ -13122,6 +13212,12 @@
       </c>
       <c r="D273">
         <v>2</v>
+      </c>
+      <c r="F273">
+        <v>69</v>
+      </c>
+      <c r="G273">
+        <v>370</v>
       </c>
       <c r="K273">
         <v>0.1</v>

</xml_diff>